<commit_message>
Authenticate the downloads and routing
</commit_message>
<xml_diff>
--- a/Excel/trip_10.xlsx
+++ b/Excel/trip_10.xlsx
@@ -2853,7 +2853,7 @@
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="35">
-        <v>42321.0</v>
+        <v>42325.0</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>23</v>
@@ -2904,7 +2904,9 @@
         <v>28</v>
       </c>
       <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="44">
+        <v>2.0</v>
+      </c>
       <c r="G10" s="44"/>
       <c r="H10" s="44"/>
       <c r="I10" s="44"/>
@@ -3143,9 +3145,7 @@
       </c>
       <c r="D19" s="41"/>
       <c r="E19" s="43"/>
-      <c r="F19" s="44">
-        <v>4.0</v>
-      </c>
+      <c r="F19" s="44"/>
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="I19" s="44"/>

</xml_diff>